<commit_message>
Applet support and SPIF changes
</commit_message>
<xml_diff>
--- a/doc/ASIC.xlsx
+++ b/doc/ASIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apps\chad\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDCA70-6FAC-47B5-B839-EB046CC06177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E1C946-47DA-4B41-9F21-6BF23B62D77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="300" windowWidth="14415" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="840" windowWidth="14415" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>WLCSP die calc</t>
   </si>
@@ -64,14 +64,31 @@
   </si>
   <si>
     <t>Wafer R</t>
+  </si>
+  <si>
+    <t>$/pin</t>
+  </si>
+  <si>
+    <t>c/mm2 =</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +116,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,20 +410,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -408,7 +441,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -422,24 +455,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -455,33 +491,41 @@
         <f>(B6+0.1)^2</f>
         <v>13.690000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f>$E$3*D6/(3.1416*$E$4^2)</f>
         <v>1.4185065598208983</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <f>E6/A6^2</f>
+        <v>2.2164164997201537E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B16" si="0">(A7+1)*$B$4</f>
+        <f t="shared" ref="B7:B15" si="0">(A7+1)*$B$4</f>
         <v>4</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C16" si="1">0.6 +$B$3*(((A7^2)/4)-1)</f>
+        <f t="shared" ref="C7:C15" si="1">0.6 +$B$3*(((A7^2)/4)-1)</f>
         <v>2.3325</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D15" si="2">(B7+0.1)^2</f>
         <v>16.809999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" ref="E7:E15" si="3">$E$3*D7/(3.1416*$E$4^2)</f>
         <v>1.7417892820006788</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F15" si="4">E7/A7^2</f>
+        <v>2.1503571382724431E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -497,12 +541,16 @@
         <f t="shared" si="2"/>
         <v>20.25</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="3"/>
         <v>2.0982292064553092</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0982292064553092E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -518,12 +566,16 @@
         <f t="shared" si="2"/>
         <v>24.010000000000005</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="3"/>
         <v>2.4878263331847896</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0560548208138758E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -539,12 +591,16 @@
         <f t="shared" si="2"/>
         <v>28.09</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="3"/>
         <v>2.9105806621891182</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0212365709646653E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -560,12 +616,16 @@
         <f t="shared" si="2"/>
         <v>32.49</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="3"/>
         <v>3.3664921934682965</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9920072150699981E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
@@ -581,12 +641,16 @@
         <f t="shared" si="2"/>
         <v>37.209999999999994</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="3"/>
         <v>3.8555609270223234</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9671229219501651E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -602,12 +666,16 @@
         <f t="shared" si="2"/>
         <v>42.25</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="3"/>
         <v>4.3777868628512007</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9456830501560891E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
@@ -623,12 +691,16 @@
         <f t="shared" si="2"/>
         <v>47.610000000000007</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f t="shared" si="3"/>
         <v>4.9331700009549282</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9270195316230188E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>18</v>
       </c>
@@ -644,12 +716,156 @@
         <f t="shared" si="2"/>
         <v>59.290000000000006</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <f t="shared" si="3"/>
         <v>6.1434078839869288</v>
       </c>
+      <c r="F15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8961135444404101E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <f>A20/B$19</f>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="C20">
+        <f>SQRT(B20)-0.7</f>
+        <v>0.49522860933439361</v>
+      </c>
+      <c r="D20">
+        <f>C20^2</f>
+        <v>0.24525137550327744</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:B26" si="5">A21/B$19</f>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C26" si="6">SQRT(B21)-0.7</f>
+        <v>0.81185789203690883</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D26" si="7">C21^2</f>
+        <v>0.65911323686261314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="5"/>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="6"/>
+        <v>1.0728105208558367</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="7"/>
+        <v>1.1509224136589717</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>64</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="5"/>
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="6"/>
+        <v>1.4380899352993952</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="7"/>
+        <v>2.0681026620094185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>88</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="5"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="6"/>
+        <v>1.8071326821120348</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>3.2657285307574369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="5"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="6"/>
+        <v>1.9726124191242438</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="7"/>
+        <v>3.8911997560832012</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>144</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="5"/>
+        <v>10.285714285714286</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="6"/>
+        <v>2.507134902949093</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="7"/>
+        <v>6.2857254215855578</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>